<commit_message>
working with my custom methods
</commit_message>
<xml_diff>
--- a/KeywordDrivenTest/TestData/Locators.xlsx
+++ b/KeywordDrivenTest/TestData/Locators.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{561BD559-53ED-409B-88E5-41177FFD51D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B91F09A9-5801-4F3B-A549-4014BFDC280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,15 +31,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>locatorName</t>
-  </si>
-  <si>
-    <t>locatorType</t>
-  </si>
-  <si>
-    <t>locator</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t>LocatorName</t>
+  </si>
+  <si>
+    <t>ElementType</t>
+  </si>
+  <si>
+    <t>LocatorType</t>
+  </si>
+  <si>
+    <t>Locator</t>
   </si>
   <si>
     <t>usernameField</t>
@@ -63,7 +66,7 @@
     <t>xpath</t>
   </si>
   <si>
-    <t>//*[@id='LoginForm']/div[5]/div/button</t>
+    <t>E</t>
   </si>
   <si>
     <t>welcomeMessage</t>
@@ -453,20 +456,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,49 +480,52 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
         <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>